<commit_message>
tweeks to graphs to make them the same size.
</commit_message>
<xml_diff>
--- a/Studies/Ketogenic Diet/Energy Output/VO2max Testing/My Vo2 max tests/VO2max-2018-05-04/VO2Max Testing DGG-2018-05-04-2.xlsx
+++ b/Studies/Ketogenic Diet/Energy Output/VO2max Testing/My Vo2 max tests/VO2max-2018-05-04/VO2Max Testing DGG-2018-05-04-2.xlsx
@@ -4,18 +4,18 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="180" windowWidth="25875" windowHeight="10740" activeTab="6"/>
+    <workbookView xWindow="360" yWindow="240" windowWidth="25875" windowHeight="10680" activeTab="6"/>
   </bookViews>
   <sheets>
-    <sheet name="vo2" sheetId="1" r:id="rId1"/>
+    <sheet name="VO2max" sheetId="1" r:id="rId1"/>
     <sheet name="VO2Perc_HR" sheetId="2" r:id="rId2"/>
-    <sheet name="FAT-OX_HR" sheetId="3" r:id="rId3"/>
-    <sheet name="CHO-OX_HR" sheetId="4" r:id="rId4"/>
+    <sheet name="FAT-OX(g)_HR" sheetId="3" r:id="rId3"/>
+    <sheet name="CHO-OX(g)_HR" sheetId="4" r:id="rId4"/>
     <sheet name="CHO-FAT_HR" sheetId="5" r:id="rId5"/>
     <sheet name="CHR-FAT_HR" sheetId="6" r:id="rId6"/>
-    <sheet name="CHR-FAT_VO2max" sheetId="7" r:id="rId7"/>
+    <sheet name="CHR-FAT(c)_VO2max" sheetId="7" r:id="rId7"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="145621"/>
 </workbook>
 </file>
 
@@ -1034,11 +1034,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="59991552"/>
-        <c:axId val="59980032"/>
+        <c:axId val="49090560"/>
+        <c:axId val="49092096"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="59991552"/>
+        <c:axId val="49090560"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="180"/>
@@ -1052,12 +1052,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="59980032"/>
+        <c:crossAx val="49092096"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="59980032"/>
+        <c:axId val="49092096"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1069,7 +1069,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="59991552"/>
+        <c:crossAx val="49090560"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1172,7 +1172,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>'FAT-OX_HR'!$B$1</c:f>
+              <c:f>'FAT-OX(g)_HR'!$B$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1195,8 +1195,8 @@
             <c:trendlineLbl>
               <c:layout>
                 <c:manualLayout>
-                  <c:x val="-8.9570335622940755E-2"/>
-                  <c:y val="-2.9918855622022692E-3"/>
+                  <c:x val="-0.15032586884086296"/>
+                  <c:y val="-6.5213653556403683E-2"/>
                 </c:manualLayout>
               </c:layout>
               <c:tx>
@@ -1250,7 +1250,7 @@
           </c:trendline>
           <c:xVal>
             <c:numRef>
-              <c:f>'FAT-OX_HR'!$A$2:$A$36</c:f>
+              <c:f>'FAT-OX(g)_HR'!$A$2:$A$36</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="35"/>
@@ -1364,7 +1364,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'FAT-OX_HR'!$B$2:$B$36</c:f>
+              <c:f>'FAT-OX(g)_HR'!$B$2:$B$36</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="35"/>
@@ -1486,14 +1486,15 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="98201600"/>
-        <c:axId val="98183424"/>
+        <c:axId val="49138304"/>
+        <c:axId val="49144192"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="98201600"/>
+        <c:axId val="49138304"/>
         <c:scaling>
           <c:orientation val="minMax"/>
-          <c:min val="60"/>
+          <c:max val="170"/>
+          <c:min val="70"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
@@ -1503,12 +1504,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="98183424"/>
+        <c:crossAx val="49144192"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="98183424"/>
+        <c:axId val="49144192"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="0"/>
@@ -1517,11 +1518,11 @@
         <c:axPos val="l"/>
         <c:majorGridlines/>
         <c:minorGridlines/>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:numFmt formatCode="#,##0.0" sourceLinked="0"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="98201600"/>
+        <c:crossAx val="49138304"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1532,8 +1533,8 @@
         <c:manualLayout>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.35553619627333816"/>
-          <c:y val="0.59102572648894525"/>
+          <c:x val="0.34607993149792449"/>
+          <c:y val="0.52515199082186181"/>
           <c:w val="0.14895552949498334"/>
           <c:h val="0.14719523695814338"/>
         </c:manualLayout>
@@ -1608,7 +1609,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>'CHO-OX_HR'!$B$1</c:f>
+              <c:f>'CHO-OX(g)_HR'!$B$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1686,7 +1687,7 @@
           </c:trendline>
           <c:xVal>
             <c:numRef>
-              <c:f>'CHO-OX_HR'!$A$2:$A$42</c:f>
+              <c:f>'CHO-OX(g)_HR'!$A$2:$A$42</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="41"/>
@@ -1818,7 +1819,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'CHO-OX_HR'!$B$2:$B$42</c:f>
+              <c:f>'CHO-OX(g)_HR'!$B$2:$B$42</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="41"/>
@@ -1958,14 +1959,15 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="66062592"/>
-        <c:axId val="66061056"/>
+        <c:axId val="49346816"/>
+        <c:axId val="49414144"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="66062592"/>
+        <c:axId val="49346816"/>
         <c:scaling>
           <c:orientation val="minMax"/>
-          <c:min val="60"/>
+          <c:max val="180"/>
+          <c:min val="70"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
@@ -1975,12 +1977,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="66061056"/>
+        <c:crossAx val="49414144"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="66061056"/>
+        <c:axId val="49414144"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1988,11 +1990,11 @@
         <c:axPos val="l"/>
         <c:majorGridlines/>
         <c:minorGridlines/>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:numFmt formatCode="#,##0.0" sourceLinked="0"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="66062592"/>
+        <c:crossAx val="49346816"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2441,8 +2443,8 @@
             <c:trendlineLbl>
               <c:layout>
                 <c:manualLayout>
-                  <c:x val="-4.802829629821808E-2"/>
-                  <c:y val="-1.3274846601385663E-2"/>
+                  <c:x val="-6.9468883961413014E-2"/>
+                  <c:y val="9.9712511184985642E-2"/>
                 </c:manualLayout>
               </c:layout>
               <c:tx>
@@ -2768,27 +2770,29 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="57928320"/>
-        <c:axId val="57926784"/>
+        <c:axId val="49455488"/>
+        <c:axId val="49457024"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="57928320"/>
+        <c:axId val="49455488"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="60"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
+        <c:majorGridlines/>
+        <c:minorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="57926784"/>
+        <c:crossAx val="49457024"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="57926784"/>
+        <c:axId val="49457024"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="6"/>
@@ -2802,7 +2806,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="57928320"/>
+        <c:crossAx val="49455488"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -3558,11 +3562,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="110174592"/>
-        <c:axId val="80460416"/>
+        <c:axId val="50342912"/>
+        <c:axId val="50356992"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="110174592"/>
+        <c:axId val="50342912"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="60"/>
@@ -3574,12 +3578,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="80460416"/>
+        <c:crossAx val="50356992"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="80460416"/>
+        <c:axId val="50356992"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3591,7 +3595,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="110174592"/>
+        <c:crossAx val="50342912"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -3652,7 +3656,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>'CHR-FAT_VO2max'!$B$1</c:f>
+              <c:f>'CHR-FAT(c)_VO2max'!$B$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -3688,7 +3692,7 @@
           </c:trendline>
           <c:xVal>
             <c:numRef>
-              <c:f>'CHR-FAT_VO2max'!$A$2:$A$42</c:f>
+              <c:f>'CHR-FAT(c)_VO2max'!$A$2:$A$42</c:f>
               <c:numCache>
                 <c:formatCode>0%</c:formatCode>
                 <c:ptCount val="41"/>
@@ -3808,7 +3812,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'CHR-FAT_VO2max'!$B$2:$B$42</c:f>
+              <c:f>'CHR-FAT(c)_VO2max'!$B$2:$B$42</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="41"/>
@@ -3933,7 +3937,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>'CHR-FAT_VO2max'!$C$1</c:f>
+              <c:f>'CHR-FAT(c)_VO2max'!$C$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -3969,7 +3973,7 @@
           </c:trendline>
           <c:xVal>
             <c:numRef>
-              <c:f>'CHR-FAT_VO2max'!$A$2:$A$42</c:f>
+              <c:f>'CHR-FAT(c)_VO2max'!$A$2:$A$42</c:f>
               <c:numCache>
                 <c:formatCode>0%</c:formatCode>
                 <c:ptCount val="41"/>
@@ -4089,7 +4093,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'CHR-FAT_VO2max'!$C$2:$C$42</c:f>
+              <c:f>'CHR-FAT(c)_VO2max'!$C$2:$C$42</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="41"/>
@@ -4217,11 +4221,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="50318720"/>
-        <c:axId val="50317184"/>
+        <c:axId val="50070656"/>
+        <c:axId val="50072192"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="50318720"/>
+        <c:axId val="50070656"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4233,12 +4237,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="50317184"/>
+        <c:crossAx val="50072192"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="50317184"/>
+        <c:axId val="50072192"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4250,7 +4254,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="50318720"/>
+        <c:crossAx val="50070656"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -4285,14 +4289,14 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>600074</xdr:colOff>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>609599</xdr:colOff>
       <xdr:row>0</xdr:row>
       <xdr:rowOff>185737</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>13</xdr:col>
-      <xdr:colOff>533400</xdr:colOff>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>542925</xdr:colOff>
       <xdr:row>29</xdr:row>
       <xdr:rowOff>161925</xdr:rowOff>
     </xdr:to>
@@ -4320,16 +4324,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>561974</xdr:colOff>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>590548</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>33336</xdr:rowOff>
+      <xdr:rowOff>176211</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>13</xdr:col>
-      <xdr:colOff>571499</xdr:colOff>
-      <xdr:row>27</xdr:row>
-      <xdr:rowOff>95249</xdr:rowOff>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>561975</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -4355,16 +4359,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>428625</xdr:colOff>
-      <xdr:row>13</xdr:row>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>19049</xdr:colOff>
+      <xdr:row>0</xdr:row>
       <xdr:rowOff>176211</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>13</xdr:col>
-      <xdr:colOff>276225</xdr:colOff>
-      <xdr:row>40</xdr:row>
-      <xdr:rowOff>161924</xdr:rowOff>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>9524</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>133350</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -4391,15 +4395,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>104774</xdr:colOff>
-      <xdr:row>0</xdr:row>
-      <xdr:rowOff>166686</xdr:rowOff>
+      <xdr:colOff>1</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>33336</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>13</xdr:col>
-      <xdr:colOff>400049</xdr:colOff>
-      <xdr:row>26</xdr:row>
-      <xdr:rowOff>95249</xdr:rowOff>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>1</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>161925</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -4426,15 +4430,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>28574</xdr:colOff>
-      <xdr:row>3</xdr:row>
-      <xdr:rowOff>157161</xdr:rowOff>
+      <xdr:colOff>9525</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>185737</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>17</xdr:col>
-      <xdr:colOff>209549</xdr:colOff>
-      <xdr:row>38</xdr:row>
-      <xdr:rowOff>38100</xdr:rowOff>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>571501</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>1</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -4461,15 +4465,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>304799</xdr:colOff>
+      <xdr:colOff>600074</xdr:colOff>
       <xdr:row>1</xdr:row>
-      <xdr:rowOff>14286</xdr:rowOff>
+      <xdr:rowOff>52386</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>17</xdr:col>
-      <xdr:colOff>219075</xdr:colOff>
-      <xdr:row>33</xdr:row>
-      <xdr:rowOff>133350</xdr:rowOff>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>19050</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -4781,7 +4785,7 @@
   <dimension ref="A1:W45"/>
   <sheetViews>
     <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="U5" sqref="U5"/>
+      <selection activeCell="E21" sqref="E21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7896,7 +7900,7 @@
   <dimension ref="A1:B38"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:B38"/>
+      <selection activeCell="G35" sqref="G35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7907,382 +7911,382 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="str">
-        <f>'vo2'!M4</f>
+        <f>VO2max!M4</f>
         <v>HR
 bpm</v>
       </c>
       <c r="B1" t="str">
-        <f>'vo2'!W4</f>
+        <f>VO2max!W4</f>
         <v>%VO2max</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2">
-        <f>'vo2'!M5</f>
+        <f>VO2max!M5</f>
         <v>78</v>
       </c>
       <c r="B2" s="4">
-        <f>'vo2'!W5</f>
+        <f>VO2max!W5</f>
         <v>0.12280701754385964</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3">
-        <f>'vo2'!M6</f>
+        <f>VO2max!M6</f>
         <v>76</v>
       </c>
       <c r="B3" s="4">
-        <f>'vo2'!W6</f>
+        <f>VO2max!W6</f>
         <v>9.0643274853801165E-2</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4">
-        <f>'vo2'!M7</f>
+        <f>VO2max!M7</f>
         <v>70</v>
       </c>
       <c r="B4" s="4">
-        <f>'vo2'!W7</f>
+        <f>VO2max!W7</f>
         <v>0.10818713450292397</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5">
-        <f>'vo2'!M8</f>
+        <f>VO2max!M8</f>
         <v>80</v>
       </c>
       <c r="B5" s="4">
-        <f>'vo2'!W8</f>
+        <f>VO2max!W8</f>
         <v>9.6491228070175419E-2</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6">
-        <f>'vo2'!M9</f>
+        <f>VO2max!M9</f>
         <v>84</v>
       </c>
       <c r="B6" s="4">
-        <f>'vo2'!W9</f>
+        <f>VO2max!W9</f>
         <v>0.10526315789473684</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7">
-        <f>'vo2'!M10</f>
+        <f>VO2max!M10</f>
         <v>76</v>
       </c>
       <c r="B7" s="4">
-        <f>'vo2'!W10</f>
+        <f>VO2max!W10</f>
         <v>0.11695906432748537</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8">
-        <f>'vo2'!M11</f>
+        <f>VO2max!M11</f>
         <v>84</v>
       </c>
       <c r="B8" s="4">
-        <f>'vo2'!W11</f>
+        <f>VO2max!W11</f>
         <v>0.17251461988304093</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9">
-        <f>'vo2'!M12</f>
+        <f>VO2max!M12</f>
         <v>92</v>
       </c>
       <c r="B9" s="4">
-        <f>'vo2'!W12</f>
+        <f>VO2max!W12</f>
         <v>0.20760233918128651</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10">
-        <f>'vo2'!M13</f>
+        <f>VO2max!M13</f>
         <v>84</v>
       </c>
       <c r="B10" s="4">
-        <f>'vo2'!W13</f>
+        <f>VO2max!W13</f>
         <v>0.16666666666666666</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11">
-        <f>'vo2'!M14</f>
+        <f>VO2max!M14</f>
         <v>82</v>
       </c>
       <c r="B11" s="4">
-        <f>'vo2'!W14</f>
+        <f>VO2max!W14</f>
         <v>0.17251461988304093</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12">
-        <f>'vo2'!M15</f>
+        <f>VO2max!M15</f>
         <v>88</v>
       </c>
       <c r="B12" s="4">
-        <f>'vo2'!W15</f>
+        <f>VO2max!W15</f>
         <v>0.22807017543859648</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13">
-        <f>'vo2'!M16</f>
+        <f>VO2max!M16</f>
         <v>88</v>
       </c>
       <c r="B13" s="4">
-        <f>'vo2'!W16</f>
+        <f>VO2max!W16</f>
         <v>0.22807017543859648</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14">
-        <f>'vo2'!M17</f>
+        <f>VO2max!M17</f>
         <v>90</v>
       </c>
       <c r="B14" s="4">
-        <f>'vo2'!W17</f>
+        <f>VO2max!W17</f>
         <v>0.27777777777777773</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15">
-        <f>'vo2'!M18</f>
+        <f>VO2max!M18</f>
         <v>94</v>
       </c>
       <c r="B15" s="4">
-        <f>'vo2'!W18</f>
+        <f>VO2max!W18</f>
         <v>0.27192982456140352</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16">
-        <f>'vo2'!M19</f>
+        <f>VO2max!M19</f>
         <v>96</v>
       </c>
       <c r="B16" s="4">
-        <f>'vo2'!W19</f>
+        <f>VO2max!W19</f>
         <v>0.34795321637426901</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17">
-        <f>'vo2'!M20</f>
+        <f>VO2max!M20</f>
         <v>99</v>
       </c>
       <c r="B17" s="4">
-        <f>'vo2'!W20</f>
+        <f>VO2max!W20</f>
         <v>0.41812865497076024</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18">
-        <f>'vo2'!M21</f>
+        <f>VO2max!M21</f>
         <v>102</v>
       </c>
       <c r="B18" s="4">
-        <f>'vo2'!W21</f>
+        <f>VO2max!W21</f>
         <v>0.40350877192982454</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19">
-        <f>'vo2'!M22</f>
+        <f>VO2max!M22</f>
         <v>103</v>
       </c>
       <c r="B19" s="4">
-        <f>'vo2'!W22</f>
+        <f>VO2max!W22</f>
         <v>0.48538011695906436</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20">
-        <f>'vo2'!M23</f>
+        <f>VO2max!M23</f>
         <v>106</v>
       </c>
       <c r="B20" s="4">
-        <f>'vo2'!W23</f>
+        <f>VO2max!W23</f>
         <v>0.48245614035087714</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21">
-        <f>'vo2'!M24</f>
+        <f>VO2max!M24</f>
         <v>114</v>
       </c>
       <c r="B21" s="4">
-        <f>'vo2'!W24</f>
+        <f>VO2max!W24</f>
         <v>0.42690058479532161</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22">
-        <f>'vo2'!M25</f>
+        <f>VO2max!M25</f>
         <v>106</v>
       </c>
       <c r="B22" s="4">
-        <f>'vo2'!W25</f>
+        <f>VO2max!W25</f>
         <v>0.49122807017543857</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23">
-        <f>'vo2'!M26</f>
+        <f>VO2max!M26</f>
         <v>109</v>
       </c>
       <c r="B23" s="4">
-        <f>'vo2'!W26</f>
+        <f>VO2max!W26</f>
         <v>0.58771929824561397</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24">
-        <f>'vo2'!M27</f>
+        <f>VO2max!M27</f>
         <v>117</v>
       </c>
       <c r="B24" s="4">
-        <f>'vo2'!W27</f>
+        <f>VO2max!W27</f>
         <v>0.62573099415204669</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25">
-        <f>'vo2'!M28</f>
+        <f>VO2max!M28</f>
         <v>124</v>
       </c>
       <c r="B25" s="4">
-        <f>'vo2'!W28</f>
+        <f>VO2max!W28</f>
         <v>0.67836257309941517</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26">
-        <f>'vo2'!M29</f>
+        <f>VO2max!M29</f>
         <v>126</v>
       </c>
       <c r="B26" s="4">
-        <f>'vo2'!W29</f>
+        <f>VO2max!W29</f>
         <v>0.62280701754385959</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27">
-        <f>'vo2'!M30</f>
+        <f>VO2max!M30</f>
         <v>129</v>
       </c>
       <c r="B27" s="4">
-        <f>'vo2'!W30</f>
+        <f>VO2max!W30</f>
         <v>0.64912280701754377</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A28">
-        <f>'vo2'!M31</f>
+        <f>VO2max!M31</f>
         <v>135</v>
       </c>
       <c r="B28" s="4">
-        <f>'vo2'!W31</f>
+        <f>VO2max!W31</f>
         <v>0.76608187134502914</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A29">
-        <f>'vo2'!M32</f>
+        <f>VO2max!M32</f>
         <v>138</v>
       </c>
       <c r="B29" s="4">
-        <f>'vo2'!W32</f>
+        <f>VO2max!W32</f>
         <v>0.72514619883040932</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A30">
-        <f>'vo2'!M33</f>
+        <f>VO2max!M33</f>
         <v>148</v>
       </c>
       <c r="B30" s="4">
-        <f>'vo2'!W33</f>
+        <f>VO2max!W33</f>
         <v>0.78070175438596479</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A31">
-        <f>'vo2'!M34</f>
+        <f>VO2max!M34</f>
         <v>139</v>
       </c>
       <c r="B31" s="4">
-        <f>'vo2'!W34</f>
+        <f>VO2max!W34</f>
         <v>0.7192982456140351</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A32">
-        <f>'vo2'!M35</f>
+        <f>VO2max!M35</f>
         <v>143</v>
       </c>
       <c r="B32" s="4">
-        <f>'vo2'!W35</f>
+        <f>VO2max!W35</f>
         <v>0.85964912280701744</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A33">
-        <f>'vo2'!M36</f>
+        <f>VO2max!M36</f>
         <v>149</v>
       </c>
       <c r="B33" s="4">
-        <f>'vo2'!W36</f>
+        <f>VO2max!W36</f>
         <v>0.85964912280701744</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A34">
-        <f>'vo2'!M37</f>
+        <f>VO2max!M37</f>
         <v>155</v>
       </c>
       <c r="B34" s="4">
-        <f>'vo2'!W37</f>
+        <f>VO2max!W37</f>
         <v>0.86257309941520466</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A35">
-        <f>'vo2'!M38</f>
+        <f>VO2max!M38</f>
         <v>158</v>
       </c>
       <c r="B35" s="4">
-        <f>'vo2'!W38</f>
+        <f>VO2max!W38</f>
         <v>0.95614035087719296</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A36">
-        <f>'vo2'!M39</f>
+        <f>VO2max!M39</f>
         <v>161</v>
       </c>
       <c r="B36" s="4">
-        <f>'vo2'!W39</f>
+        <f>VO2max!W39</f>
         <v>0.9385964912280701</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A37">
-        <f>'vo2'!M40</f>
+        <f>VO2max!M40</f>
         <v>165</v>
       </c>
       <c r="B37" s="4">
-        <f>'vo2'!W40</f>
+        <f>VO2max!W40</f>
         <v>0.97076023391812871</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A38">
-        <f>'vo2'!M41</f>
+        <f>VO2max!M41</f>
         <v>167</v>
       </c>
       <c r="B38" s="4">
-        <f>'vo2'!W41</f>
+        <f>VO2max!W41</f>
         <v>1</v>
       </c>
     </row>
@@ -8297,374 +8301,374 @@
   <dimension ref="A1:B36"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:B36"/>
+      <selection activeCell="D1" sqref="D1:O1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="8.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="str">
-        <f>'vo2'!M4</f>
+        <f>VO2max!M4</f>
         <v>HR
 bpm</v>
       </c>
       <c r="B1" t="str">
-        <f>'vo2'!T4</f>
+        <f>VO2max!T4</f>
         <v>FatOx 
 (g/min)</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2">
-        <f>'vo2'!M5</f>
+        <f>VO2max!M5</f>
         <v>78</v>
       </c>
       <c r="B2">
-        <f>'vo2'!T5</f>
+        <f>VO2max!T5</f>
         <v>0.216144</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3">
-        <f>'vo2'!M6</f>
+        <f>VO2max!M6</f>
         <v>76</v>
       </c>
       <c r="B3">
-        <f>'vo2'!T6</f>
+        <f>VO2max!T6</f>
         <v>0.13434666666666661</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4">
-        <f>'vo2'!M7</f>
+        <f>VO2max!M7</f>
         <v>70</v>
       </c>
       <c r="B4">
-        <f>'vo2'!T7</f>
+        <f>VO2max!T7</f>
         <v>0.14940799999999993</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5">
-        <f>'vo2'!M8</f>
+        <f>VO2max!M8</f>
         <v>80</v>
       </c>
       <c r="B5">
-        <f>'vo2'!T8</f>
+        <f>VO2max!T8</f>
         <v>0.15654399999999996</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6">
-        <f>'vo2'!M9</f>
+        <f>VO2max!M9</f>
         <v>84</v>
       </c>
       <c r="B6">
-        <f>'vo2'!T9</f>
+        <f>VO2max!T9</f>
         <v>0.18345599999999995</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7">
-        <f>'vo2'!M10</f>
+        <f>VO2max!M10</f>
         <v>76</v>
       </c>
       <c r="B7">
-        <f>'vo2'!T10</f>
+        <f>VO2max!T10</f>
         <v>0.18973333333333328</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8">
-        <f>'vo2'!M11</f>
+        <f>VO2max!M11</f>
         <v>84</v>
       </c>
       <c r="B8">
-        <f>'vo2'!T11</f>
+        <f>VO2max!T11</f>
         <v>0.3258826666666666</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9">
-        <f>'vo2'!M12</f>
+        <f>VO2max!M12</f>
         <v>92</v>
       </c>
       <c r="B9">
-        <f>'vo2'!T12</f>
+        <f>VO2max!T12</f>
         <v>0.39207999999999998</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10">
-        <f>'vo2'!M13</f>
+        <f>VO2max!M13</f>
         <v>84</v>
       </c>
       <c r="B10">
-        <f>'vo2'!T13</f>
+        <f>VO2max!T13</f>
         <v>0.31211733333333336</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11">
-        <f>'vo2'!M14</f>
+        <f>VO2max!M14</f>
         <v>82</v>
       </c>
       <c r="B11">
-        <f>'vo2'!T14</f>
+        <f>VO2max!T14</f>
         <v>0.37807999999999992</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12">
-        <f>'vo2'!M15</f>
+        <f>VO2max!M15</f>
         <v>88</v>
       </c>
       <c r="B12">
-        <f>'vo2'!T15</f>
+        <f>VO2max!T15</f>
         <v>0.53437866666666656</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13">
-        <f>'vo2'!M16</f>
+        <f>VO2max!M16</f>
         <v>88</v>
       </c>
       <c r="B13">
-        <f>'vo2'!T16</f>
+        <f>VO2max!T16</f>
         <v>0.54207466666666659</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14">
-        <f>'vo2'!M17</f>
+        <f>VO2max!M17</f>
         <v>90</v>
       </c>
       <c r="B14">
-        <f>'vo2'!T17</f>
+        <f>VO2max!T17</f>
         <v>0.65179199999999993</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15">
-        <f>'vo2'!M18</f>
+        <f>VO2max!M18</f>
         <v>94</v>
       </c>
       <c r="B15">
-        <f>'vo2'!T18</f>
+        <f>VO2max!T18</f>
         <v>0.65927466666666656</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16">
-        <f>'vo2'!M19</f>
+        <f>VO2max!M19</f>
         <v>96</v>
       </c>
       <c r="B16">
-        <f>'vo2'!T19</f>
+        <f>VO2max!T19</f>
         <v>0.88618666666666657</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17">
-        <f>'vo2'!M20</f>
+        <f>VO2max!M20</f>
         <v>99</v>
       </c>
       <c r="B17">
-        <f>'vo2'!T20</f>
+        <f>VO2max!T20</f>
         <v>1.0834933333333334</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18">
-        <f>'vo2'!M21</f>
+        <f>VO2max!M21</f>
         <v>102</v>
       </c>
       <c r="B18">
-        <f>'vo2'!T21</f>
+        <f>VO2max!T21</f>
         <v>1.0214399999999999</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19">
-        <f>'vo2'!M22</f>
+        <f>VO2max!M22</f>
         <v>103</v>
       </c>
       <c r="B19">
-        <f>'vo2'!T22</f>
+        <f>VO2max!T22</f>
         <v>1.2349866666666669</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20">
-        <f>'vo2'!M23</f>
+        <f>VO2max!M23</f>
         <v>106</v>
       </c>
       <c r="B20">
-        <f>'vo2'!T23</f>
+        <f>VO2max!T23</f>
         <v>1.1697920000000002</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21">
-        <f>'vo2'!M24</f>
+        <f>VO2max!M24</f>
         <v>114</v>
       </c>
       <c r="B21">
-        <f>'vo2'!T24</f>
+        <f>VO2max!T24</f>
         <v>0.98323199999999977</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22">
-        <f>'vo2'!M25</f>
+        <f>VO2max!M25</f>
         <v>106</v>
       </c>
       <c r="B22">
-        <f>'vo2'!T25</f>
+        <f>VO2max!T25</f>
         <v>1.1095466666666665</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23">
-        <f>'vo2'!M26</f>
+        <f>VO2max!M26</f>
         <v>109</v>
       </c>
       <c r="B23">
-        <f>'vo2'!T26</f>
+        <f>VO2max!T26</f>
         <v>1.3191733333333331</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24">
-        <f>'vo2'!M27</f>
+        <f>VO2max!M27</f>
         <v>117</v>
       </c>
       <c r="B24">
-        <f>'vo2'!T27</f>
+        <f>VO2max!T27</f>
         <v>1.2177599999999997</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25">
-        <f>'vo2'!M28</f>
+        <f>VO2max!M28</f>
         <v>124</v>
       </c>
       <c r="B25">
-        <f>'vo2'!T28</f>
+        <f>VO2max!T28</f>
         <v>1.1967839999999998</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26">
-        <f>'vo2'!M29</f>
+        <f>VO2max!M29</f>
         <v>126</v>
       </c>
       <c r="B26">
-        <f>'vo2'!T29</f>
+        <f>VO2max!T29</f>
         <v>1.0198666666666665</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27">
-        <f>'vo2'!M30</f>
+        <f>VO2max!M30</f>
         <v>129</v>
       </c>
       <c r="B27">
-        <f>'vo2'!T30</f>
+        <f>VO2max!T30</f>
         <v>1.071733333333333</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A28">
-        <f>'vo2'!M31</f>
+        <f>VO2max!M31</f>
         <v>135</v>
       </c>
       <c r="B28">
-        <f>'vo2'!T31</f>
+        <f>VO2max!T31</f>
         <v>1.1645973333333328</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A29">
-        <f>'vo2'!M32</f>
+        <f>VO2max!M32</f>
         <v>138</v>
       </c>
       <c r="B29">
-        <f>'vo2'!T32</f>
+        <f>VO2max!T32</f>
         <v>0.8702399999999999</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A30">
-        <f>'vo2'!M33</f>
+        <f>VO2max!M33</f>
         <v>148</v>
       </c>
       <c r="B30">
-        <f>'vo2'!T33</f>
+        <f>VO2max!T33</f>
         <v>0.89089066666666661</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A31">
-        <f>'vo2'!M34</f>
+        <f>VO2max!M34</f>
         <v>139</v>
       </c>
       <c r="B31">
-        <f>'vo2'!T34</f>
+        <f>VO2max!T34</f>
         <v>0.77303466666666654</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A32">
-        <f>'vo2'!M35</f>
+        <f>VO2max!M35</f>
         <v>143</v>
       </c>
       <c r="B32">
-        <f>'vo2'!T35</f>
+        <f>VO2max!T35</f>
         <v>0.92194133333333306</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A33">
-        <f>'vo2'!M36</f>
+        <f>VO2max!M36</f>
         <v>149</v>
       </c>
       <c r="B33">
-        <f>'vo2'!T36</f>
+        <f>VO2max!T36</f>
         <v>0.58383999999999947</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A34">
-        <f>'vo2'!M37</f>
+        <f>VO2max!M37</f>
         <v>155</v>
       </c>
       <c r="B34">
-        <f>'vo2'!T37</f>
+        <f>VO2max!T37</f>
         <v>0.41488533333333255</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A35">
-        <f>'vo2'!M38</f>
+        <f>VO2max!M38</f>
         <v>158</v>
       </c>
       <c r="B35">
-        <f>'vo2'!T38</f>
+        <f>VO2max!T38</f>
         <v>0.26408533333333328</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A36">
-        <f>'vo2'!M39</f>
+        <f>VO2max!M39</f>
         <v>161</v>
       </c>
       <c r="B36">
-        <f>'vo2'!T39</f>
+        <f>VO2max!T39</f>
         <v>6.5274666666666425E-2</v>
       </c>
     </row>
@@ -8678,431 +8682,435 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B42"/>
   <sheetViews>
-    <sheetView topLeftCell="A14" workbookViewId="0">
-      <selection sqref="A1:B42"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H32" sqref="H32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="8.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.28515625" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="str">
-        <f>'vo2'!M4</f>
+        <f>VO2max!M4</f>
         <v>HR
 bpm</v>
       </c>
       <c r="B1" t="str">
-        <f>'vo2'!U4</f>
+        <f>VO2max!U4</f>
         <v>ChoOx 
 (g/min)</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2">
-        <f>'vo2'!M5</f>
+        <f>VO2max!M5</f>
         <v>78</v>
       </c>
       <c r="B2">
-        <f>'vo2'!U5</f>
+        <f>VO2max!U5</f>
         <v>5.4036000000000056E-2</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3">
-        <f>'vo2'!M6</f>
+        <f>VO2max!M6</f>
         <v>76</v>
       </c>
       <c r="B3">
-        <f>'vo2'!U6</f>
+        <f>VO2max!U6</f>
         <v>0.10992000000000011</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4">
-        <f>'vo2'!M7</f>
+        <f>VO2max!M7</f>
         <v>70</v>
       </c>
       <c r="B4">
-        <f>'vo2'!U7</f>
+        <f>VO2max!U7</f>
         <v>0.14407200000000012</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5">
-        <f>'vo2'!M8</f>
+        <f>VO2max!M8</f>
         <v>80</v>
       </c>
       <c r="B5">
-        <f>'vo2'!U8</f>
+        <f>VO2max!U8</f>
         <v>8.8056000000000079E-2</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6">
-        <f>'vo2'!M9</f>
+        <f>VO2max!M9</f>
         <v>84</v>
       </c>
       <c r="B6">
-        <f>'vo2'!U9</f>
+        <f>VO2max!U9</f>
         <v>6.3504000000000102E-2</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7">
-        <f>'vo2'!M10</f>
+        <f>VO2max!M10</f>
         <v>76</v>
       </c>
       <c r="B7">
-        <f>'vo2'!U10</f>
+        <f>VO2max!U10</f>
         <v>8.5380000000000081E-2</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8">
-        <f>'vo2'!M11</f>
+        <f>VO2max!M11</f>
         <v>84</v>
       </c>
       <c r="B8">
-        <f>'vo2'!U11</f>
+        <f>VO2max!U11</f>
         <v>2.5283999999999991E-2</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9">
-        <f>'vo2'!M12</f>
+        <f>VO2max!M12</f>
         <v>92</v>
       </c>
       <c r="B9">
-        <f>'vo2'!U12</f>
+        <f>VO2max!U12</f>
         <v>3.0419999999999992E-2</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10">
-        <f>'vo2'!M13</f>
+        <f>VO2max!M13</f>
         <v>84</v>
       </c>
       <c r="B10">
-        <f>'vo2'!U13</f>
+        <f>VO2max!U13</f>
         <v>2.4215999999999994E-2</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11">
-        <f>'vo2'!M14</f>
+        <f>VO2max!M14</f>
         <v>82</v>
       </c>
       <c r="B11">
-        <f>'vo2'!U14</f>
+        <f>VO2max!U14</f>
         <v>-0.10007999999999981</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12">
-        <f>'vo2'!M15</f>
+        <f>VO2max!M15</f>
         <v>88</v>
       </c>
       <c r="B12">
-        <f>'vo2'!U15</f>
+        <f>VO2max!U15</f>
         <v>-0.22747199999999981</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13">
-        <f>'vo2'!M16</f>
+        <f>VO2max!M16</f>
         <v>88</v>
       </c>
       <c r="B13">
-        <f>'vo2'!U16</f>
+        <f>VO2max!U16</f>
         <v>-0.23074799999999981</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14">
-        <f>'vo2'!M17</f>
+        <f>VO2max!M17</f>
         <v>90</v>
       </c>
       <c r="B14">
-        <f>'vo2'!U17</f>
+        <f>VO2max!U17</f>
         <v>-0.27745199999999981</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15">
-        <f>'vo2'!M18</f>
+        <f>VO2max!M18</f>
         <v>94</v>
       </c>
       <c r="B15">
-        <f>'vo2'!U18</f>
+        <f>VO2max!U18</f>
         <v>-0.3122879999999999</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16">
-        <f>'vo2'!M19</f>
+        <f>VO2max!M19</f>
         <v>96</v>
       </c>
       <c r="B16">
-        <f>'vo2'!U19</f>
+        <f>VO2max!U19</f>
         <v>-0.49847999999999987</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17">
-        <f>'vo2'!M20</f>
+        <f>VO2max!M20</f>
         <v>99</v>
       </c>
       <c r="B17">
-        <f>'vo2'!U20</f>
+        <f>VO2max!U20</f>
         <v>-0.65406000000000009</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18">
-        <f>'vo2'!M21</f>
+        <f>VO2max!M21</f>
         <v>102</v>
       </c>
       <c r="B18">
-        <f>'vo2'!U21</f>
+        <f>VO2max!U21</f>
         <v>-0.57455999999999996</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19">
-        <f>'vo2'!M22</f>
+        <f>VO2max!M22</f>
         <v>103</v>
       </c>
       <c r="B19">
-        <f>'vo2'!U22</f>
+        <f>VO2max!U22</f>
         <v>-0.69467999999999996</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20">
-        <f>'vo2'!M23</f>
+        <f>VO2max!M23</f>
         <v>106</v>
       </c>
       <c r="B20">
-        <f>'vo2'!U23</f>
+        <f>VO2max!U23</f>
         <v>-0.55411199999999994</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21">
-        <f>'vo2'!M24</f>
+        <f>VO2max!M24</f>
         <v>114</v>
       </c>
       <c r="B21">
-        <f>'vo2'!U24</f>
+        <f>VO2max!U24</f>
         <v>-0.36871199999999954</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22">
-        <f>'vo2'!M25</f>
+        <f>VO2max!M25</f>
         <v>106</v>
       </c>
       <c r="B22">
-        <f>'vo2'!U25</f>
+        <f>VO2max!U25</f>
         <v>-0.35663999999999968</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23">
-        <f>'vo2'!M26</f>
+        <f>VO2max!M26</f>
         <v>109</v>
       </c>
       <c r="B23">
-        <f>'vo2'!U26</f>
+        <f>VO2max!U26</f>
         <v>-0.42401999999999962</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24">
-        <f>'vo2'!M27</f>
+        <f>VO2max!M27</f>
         <v>117</v>
       </c>
       <c r="B24">
-        <f>'vo2'!U27</f>
+        <f>VO2max!U27</f>
         <v>0</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25">
-        <f>'vo2'!M28</f>
+        <f>VO2max!M28</f>
         <v>124</v>
       </c>
       <c r="B25">
-        <f>'vo2'!U28</f>
+        <f>VO2max!U28</f>
         <v>0.29919600000000024</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26">
-        <f>'vo2'!M29</f>
+        <f>VO2max!M29</f>
         <v>126</v>
       </c>
       <c r="B26">
-        <f>'vo2'!U29</f>
+        <f>VO2max!U29</f>
         <v>0.45894000000000057</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27">
-        <f>'vo2'!M30</f>
+        <f>VO2max!M30</f>
         <v>129</v>
       </c>
       <c r="B27">
-        <f>'vo2'!U30</f>
+        <f>VO2max!U30</f>
         <v>0.48228000000000049</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A28">
-        <f>'vo2'!M31</f>
+        <f>VO2max!M31</f>
         <v>135</v>
       </c>
       <c r="B28">
-        <f>'vo2'!U31</f>
+        <f>VO2max!U31</f>
         <v>0.79749600000000098</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A29">
-        <f>'vo2'!M32</f>
+        <f>VO2max!M32</f>
         <v>138</v>
       </c>
       <c r="B29">
-        <f>'vo2'!U32</f>
+        <f>VO2max!U32</f>
         <v>1.3053600000000001</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A30">
-        <f>'vo2'!M33</f>
+        <f>VO2max!M33</f>
         <v>148</v>
       </c>
       <c r="B30">
-        <f>'vo2'!U33</f>
+        <f>VO2max!U33</f>
         <v>1.532856</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A31">
-        <f>'vo2'!M34</f>
+        <f>VO2max!M34</f>
         <v>139</v>
       </c>
       <c r="B31">
-        <f>'vo2'!U34</f>
+        <f>VO2max!U34</f>
         <v>1.5219120000000006</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A32">
-        <f>'vo2'!M35</f>
+        <f>VO2max!M35</f>
         <v>143</v>
       </c>
       <c r="B32">
-        <f>'vo2'!U35</f>
+        <f>VO2max!U35</f>
         <v>1.8150720000000005</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A33">
-        <f>'vo2'!M36</f>
+        <f>VO2max!M36</f>
         <v>149</v>
       </c>
       <c r="B33">
-        <f>'vo2'!U36</f>
+        <f>VO2max!U36</f>
         <v>2.6272800000000012</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A34">
-        <f>'vo2'!M37</f>
+        <f>VO2max!M37</f>
         <v>155</v>
       </c>
       <c r="B34">
-        <f>'vo2'!U37</f>
+        <f>VO2max!U37</f>
         <v>3.0671880000000007</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A35">
-        <f>'vo2'!M38</f>
+        <f>VO2max!M38</f>
         <v>158</v>
       </c>
       <c r="B35">
-        <f>'vo2'!U38</f>
+        <f>VO2max!U38</f>
         <v>3.8622480000000006</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A36">
-        <f>'vo2'!M39</f>
+        <f>VO2max!M39</f>
         <v>161</v>
       </c>
       <c r="B36">
-        <f>'vo2'!U39</f>
+        <f>VO2max!U39</f>
         <v>4.2591720000000004</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A37">
-        <f>'vo2'!M40</f>
+        <f>VO2max!M40</f>
         <v>165</v>
       </c>
       <c r="B37">
-        <f>'vo2'!U40</f>
+        <f>VO2max!U40</f>
         <v>5.2264800000000022</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A38">
-        <f>'vo2'!M41</f>
+        <f>VO2max!M41</f>
         <v>167</v>
       </c>
       <c r="B38">
-        <f>'vo2'!U41</f>
+        <f>VO2max!U41</f>
         <v>5.3737680000000019</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A39">
-        <f>'vo2'!M42</f>
+        <f>VO2max!M42</f>
         <v>169</v>
       </c>
       <c r="B39">
-        <f>'vo2'!U42</f>
+        <f>VO2max!U42</f>
         <v>5.9927520000000012</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A40">
-        <f>'vo2'!M43</f>
+        <f>VO2max!M43</f>
         <v>173</v>
       </c>
       <c r="B40">
-        <f>'vo2'!U43</f>
+        <f>VO2max!U43</f>
         <v>5.0871600000000017</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A41">
-        <f>'vo2'!M44</f>
+        <f>VO2max!M44</f>
         <v>170</v>
       </c>
       <c r="B41">
-        <f>'vo2'!U44</f>
+        <f>VO2max!U44</f>
         <v>5.6129040000000012</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A42">
-        <f>'vo2'!M45</f>
+        <f>VO2max!M45</f>
         <v>161</v>
       </c>
       <c r="B42">
-        <f>'vo2'!U45</f>
+        <f>VO2max!U45</f>
         <v>3.0469560000000007</v>
       </c>
     </row>
@@ -9117,599 +9125,599 @@
   <dimension ref="A1:C42"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="P22" sqref="P22"/>
+      <selection activeCell="G34" sqref="G34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="str">
-        <f>'vo2'!M4</f>
+        <f>VO2max!M4</f>
         <v>HR
 bpm</v>
       </c>
       <c r="B1" t="str">
-        <f>'vo2'!T4</f>
+        <f>VO2max!T4</f>
         <v>FatOx 
 (g/min)</v>
       </c>
       <c r="C1" t="str">
-        <f>'vo2'!U4</f>
+        <f>VO2max!U4</f>
         <v>ChoOx 
 (g/min)</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2">
-        <f>'vo2'!M5</f>
+        <f>VO2max!M5</f>
         <v>78</v>
       </c>
       <c r="B2">
-        <f>'vo2'!T5</f>
+        <f>VO2max!T5</f>
         <v>0.216144</v>
       </c>
       <c r="C2">
-        <f>'vo2'!U5</f>
+        <f>VO2max!U5</f>
         <v>5.4036000000000056E-2</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3">
-        <f>'vo2'!M6</f>
+        <f>VO2max!M6</f>
         <v>76</v>
       </c>
       <c r="B3">
-        <f>'vo2'!T6</f>
+        <f>VO2max!T6</f>
         <v>0.13434666666666661</v>
       </c>
       <c r="C3">
-        <f>'vo2'!U6</f>
+        <f>VO2max!U6</f>
         <v>0.10992000000000011</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4">
-        <f>'vo2'!M7</f>
+        <f>VO2max!M7</f>
         <v>70</v>
       </c>
       <c r="B4">
-        <f>'vo2'!T7</f>
+        <f>VO2max!T7</f>
         <v>0.14940799999999993</v>
       </c>
       <c r="C4">
-        <f>'vo2'!U7</f>
+        <f>VO2max!U7</f>
         <v>0.14407200000000012</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5">
-        <f>'vo2'!M8</f>
+        <f>VO2max!M8</f>
         <v>80</v>
       </c>
       <c r="B5">
-        <f>'vo2'!T8</f>
+        <f>VO2max!T8</f>
         <v>0.15654399999999996</v>
       </c>
       <c r="C5">
-        <f>'vo2'!U8</f>
+        <f>VO2max!U8</f>
         <v>8.8056000000000079E-2</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6">
-        <f>'vo2'!M9</f>
+        <f>VO2max!M9</f>
         <v>84</v>
       </c>
       <c r="B6">
-        <f>'vo2'!T9</f>
+        <f>VO2max!T9</f>
         <v>0.18345599999999995</v>
       </c>
       <c r="C6">
-        <f>'vo2'!U9</f>
+        <f>VO2max!U9</f>
         <v>6.3504000000000102E-2</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7">
-        <f>'vo2'!M10</f>
+        <f>VO2max!M10</f>
         <v>76</v>
       </c>
       <c r="B7">
-        <f>'vo2'!T10</f>
+        <f>VO2max!T10</f>
         <v>0.18973333333333328</v>
       </c>
       <c r="C7">
-        <f>'vo2'!U10</f>
+        <f>VO2max!U10</f>
         <v>8.5380000000000081E-2</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8">
-        <f>'vo2'!M11</f>
+        <f>VO2max!M11</f>
         <v>84</v>
       </c>
       <c r="B8">
-        <f>'vo2'!T11</f>
+        <f>VO2max!T11</f>
         <v>0.3258826666666666</v>
       </c>
       <c r="C8">
-        <f>'vo2'!U11</f>
+        <f>VO2max!U11</f>
         <v>2.5283999999999991E-2</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9">
-        <f>'vo2'!M12</f>
+        <f>VO2max!M12</f>
         <v>92</v>
       </c>
       <c r="B9">
-        <f>'vo2'!T12</f>
+        <f>VO2max!T12</f>
         <v>0.39207999999999998</v>
       </c>
       <c r="C9">
-        <f>'vo2'!U12</f>
+        <f>VO2max!U12</f>
         <v>3.0419999999999992E-2</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10">
-        <f>'vo2'!M13</f>
+        <f>VO2max!M13</f>
         <v>84</v>
       </c>
       <c r="B10">
-        <f>'vo2'!T13</f>
+        <f>VO2max!T13</f>
         <v>0.31211733333333336</v>
       </c>
       <c r="C10">
-        <f>'vo2'!U13</f>
+        <f>VO2max!U13</f>
         <v>2.4215999999999994E-2</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11">
-        <f>'vo2'!M14</f>
+        <f>VO2max!M14</f>
         <v>82</v>
       </c>
       <c r="B11">
-        <f>'vo2'!T14</f>
+        <f>VO2max!T14</f>
         <v>0.37807999999999992</v>
       </c>
       <c r="C11">
-        <f>'vo2'!U14</f>
+        <f>VO2max!U14</f>
         <v>-0.10007999999999981</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12">
-        <f>'vo2'!M15</f>
+        <f>VO2max!M15</f>
         <v>88</v>
       </c>
       <c r="B12">
-        <f>'vo2'!T15</f>
+        <f>VO2max!T15</f>
         <v>0.53437866666666656</v>
       </c>
       <c r="C12">
-        <f>'vo2'!U15</f>
+        <f>VO2max!U15</f>
         <v>-0.22747199999999981</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13">
-        <f>'vo2'!M16</f>
+        <f>VO2max!M16</f>
         <v>88</v>
       </c>
       <c r="B13">
-        <f>'vo2'!T16</f>
+        <f>VO2max!T16</f>
         <v>0.54207466666666659</v>
       </c>
       <c r="C13">
-        <f>'vo2'!U16</f>
+        <f>VO2max!U16</f>
         <v>-0.23074799999999981</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14">
-        <f>'vo2'!M17</f>
+        <f>VO2max!M17</f>
         <v>90</v>
       </c>
       <c r="B14">
-        <f>'vo2'!T17</f>
+        <f>VO2max!T17</f>
         <v>0.65179199999999993</v>
       </c>
       <c r="C14">
-        <f>'vo2'!U17</f>
+        <f>VO2max!U17</f>
         <v>-0.27745199999999981</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15">
-        <f>'vo2'!M18</f>
+        <f>VO2max!M18</f>
         <v>94</v>
       </c>
       <c r="B15">
-        <f>'vo2'!T18</f>
+        <f>VO2max!T18</f>
         <v>0.65927466666666656</v>
       </c>
       <c r="C15">
-        <f>'vo2'!U18</f>
+        <f>VO2max!U18</f>
         <v>-0.3122879999999999</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16">
-        <f>'vo2'!M19</f>
+        <f>VO2max!M19</f>
         <v>96</v>
       </c>
       <c r="B16">
-        <f>'vo2'!T19</f>
+        <f>VO2max!T19</f>
         <v>0.88618666666666657</v>
       </c>
       <c r="C16">
-        <f>'vo2'!U19</f>
+        <f>VO2max!U19</f>
         <v>-0.49847999999999987</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17">
-        <f>'vo2'!M20</f>
+        <f>VO2max!M20</f>
         <v>99</v>
       </c>
       <c r="B17">
-        <f>'vo2'!T20</f>
+        <f>VO2max!T20</f>
         <v>1.0834933333333334</v>
       </c>
       <c r="C17">
-        <f>'vo2'!U20</f>
+        <f>VO2max!U20</f>
         <v>-0.65406000000000009</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18">
-        <f>'vo2'!M21</f>
+        <f>VO2max!M21</f>
         <v>102</v>
       </c>
       <c r="B18">
-        <f>'vo2'!T21</f>
+        <f>VO2max!T21</f>
         <v>1.0214399999999999</v>
       </c>
       <c r="C18">
-        <f>'vo2'!U21</f>
+        <f>VO2max!U21</f>
         <v>-0.57455999999999996</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19">
-        <f>'vo2'!M22</f>
+        <f>VO2max!M22</f>
         <v>103</v>
       </c>
       <c r="B19">
-        <f>'vo2'!T22</f>
+        <f>VO2max!T22</f>
         <v>1.2349866666666669</v>
       </c>
       <c r="C19">
-        <f>'vo2'!U22</f>
+        <f>VO2max!U22</f>
         <v>-0.69467999999999996</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20">
-        <f>'vo2'!M23</f>
+        <f>VO2max!M23</f>
         <v>106</v>
       </c>
       <c r="B20">
-        <f>'vo2'!T23</f>
+        <f>VO2max!T23</f>
         <v>1.1697920000000002</v>
       </c>
       <c r="C20">
-        <f>'vo2'!U23</f>
+        <f>VO2max!U23</f>
         <v>-0.55411199999999994</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21">
-        <f>'vo2'!M24</f>
+        <f>VO2max!M24</f>
         <v>114</v>
       </c>
       <c r="B21">
-        <f>'vo2'!T24</f>
+        <f>VO2max!T24</f>
         <v>0.98323199999999977</v>
       </c>
       <c r="C21">
-        <f>'vo2'!U24</f>
+        <f>VO2max!U24</f>
         <v>-0.36871199999999954</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22">
-        <f>'vo2'!M25</f>
+        <f>VO2max!M25</f>
         <v>106</v>
       </c>
       <c r="B22">
-        <f>'vo2'!T25</f>
+        <f>VO2max!T25</f>
         <v>1.1095466666666665</v>
       </c>
       <c r="C22">
-        <f>'vo2'!U25</f>
+        <f>VO2max!U25</f>
         <v>-0.35663999999999968</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23">
-        <f>'vo2'!M26</f>
+        <f>VO2max!M26</f>
         <v>109</v>
       </c>
       <c r="B23">
-        <f>'vo2'!T26</f>
+        <f>VO2max!T26</f>
         <v>1.3191733333333331</v>
       </c>
       <c r="C23">
-        <f>'vo2'!U26</f>
+        <f>VO2max!U26</f>
         <v>-0.42401999999999962</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24">
-        <f>'vo2'!M27</f>
+        <f>VO2max!M27</f>
         <v>117</v>
       </c>
       <c r="B24">
-        <f>'vo2'!T27</f>
+        <f>VO2max!T27</f>
         <v>1.2177599999999997</v>
       </c>
       <c r="C24">
-        <f>'vo2'!U27</f>
+        <f>VO2max!U27</f>
         <v>0</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25">
-        <f>'vo2'!M28</f>
+        <f>VO2max!M28</f>
         <v>124</v>
       </c>
       <c r="B25">
-        <f>'vo2'!T28</f>
+        <f>VO2max!T28</f>
         <v>1.1967839999999998</v>
       </c>
       <c r="C25">
-        <f>'vo2'!U28</f>
+        <f>VO2max!U28</f>
         <v>0.29919600000000024</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26">
-        <f>'vo2'!M29</f>
+        <f>VO2max!M29</f>
         <v>126</v>
       </c>
       <c r="B26">
-        <f>'vo2'!T29</f>
+        <f>VO2max!T29</f>
         <v>1.0198666666666665</v>
       </c>
       <c r="C26">
-        <f>'vo2'!U29</f>
+        <f>VO2max!U29</f>
         <v>0.45894000000000057</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27">
-        <f>'vo2'!M30</f>
+        <f>VO2max!M30</f>
         <v>129</v>
       </c>
       <c r="B27">
-        <f>'vo2'!T30</f>
+        <f>VO2max!T30</f>
         <v>1.071733333333333</v>
       </c>
       <c r="C27">
-        <f>'vo2'!U30</f>
+        <f>VO2max!U30</f>
         <v>0.48228000000000049</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28">
-        <f>'vo2'!M31</f>
+        <f>VO2max!M31</f>
         <v>135</v>
       </c>
       <c r="B28">
-        <f>'vo2'!T31</f>
+        <f>VO2max!T31</f>
         <v>1.1645973333333328</v>
       </c>
       <c r="C28">
-        <f>'vo2'!U31</f>
+        <f>VO2max!U31</f>
         <v>0.79749600000000098</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29">
-        <f>'vo2'!M32</f>
+        <f>VO2max!M32</f>
         <v>138</v>
       </c>
       <c r="B29">
-        <f>'vo2'!T32</f>
+        <f>VO2max!T32</f>
         <v>0.8702399999999999</v>
       </c>
       <c r="C29">
-        <f>'vo2'!U32</f>
+        <f>VO2max!U32</f>
         <v>1.3053600000000001</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30">
-        <f>'vo2'!M33</f>
+        <f>VO2max!M33</f>
         <v>148</v>
       </c>
       <c r="B30">
-        <f>'vo2'!T33</f>
+        <f>VO2max!T33</f>
         <v>0.89089066666666661</v>
       </c>
       <c r="C30">
-        <f>'vo2'!U33</f>
+        <f>VO2max!U33</f>
         <v>1.532856</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31">
-        <f>'vo2'!M34</f>
+        <f>VO2max!M34</f>
         <v>139</v>
       </c>
       <c r="B31">
-        <f>'vo2'!T34</f>
+        <f>VO2max!T34</f>
         <v>0.77303466666666654</v>
       </c>
       <c r="C31">
-        <f>'vo2'!U34</f>
+        <f>VO2max!U34</f>
         <v>1.5219120000000006</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32">
-        <f>'vo2'!M35</f>
+        <f>VO2max!M35</f>
         <v>143</v>
       </c>
       <c r="B32">
-        <f>'vo2'!T35</f>
+        <f>VO2max!T35</f>
         <v>0.92194133333333306</v>
       </c>
       <c r="C32">
-        <f>'vo2'!U35</f>
+        <f>VO2max!U35</f>
         <v>1.8150720000000005</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33">
-        <f>'vo2'!M36</f>
+        <f>VO2max!M36</f>
         <v>149</v>
       </c>
       <c r="B33">
-        <f>'vo2'!T36</f>
+        <f>VO2max!T36</f>
         <v>0.58383999999999947</v>
       </c>
       <c r="C33">
-        <f>'vo2'!U36</f>
+        <f>VO2max!U36</f>
         <v>2.6272800000000012</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A34">
-        <f>'vo2'!M37</f>
+        <f>VO2max!M37</f>
         <v>155</v>
       </c>
       <c r="B34">
-        <f>'vo2'!T37</f>
+        <f>VO2max!T37</f>
         <v>0.41488533333333255</v>
       </c>
       <c r="C34">
-        <f>'vo2'!U37</f>
+        <f>VO2max!U37</f>
         <v>3.0671880000000007</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A35">
-        <f>'vo2'!M38</f>
+        <f>VO2max!M38</f>
         <v>158</v>
       </c>
       <c r="B35">
-        <f>'vo2'!T38</f>
+        <f>VO2max!T38</f>
         <v>0.26408533333333328</v>
       </c>
       <c r="C35">
-        <f>'vo2'!U38</f>
+        <f>VO2max!U38</f>
         <v>3.8622480000000006</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A36">
-        <f>'vo2'!M39</f>
+        <f>VO2max!M39</f>
         <v>161</v>
       </c>
       <c r="B36">
-        <f>'vo2'!T39</f>
+        <f>VO2max!T39</f>
         <v>6.5274666666666425E-2</v>
       </c>
       <c r="C36">
-        <f>'vo2'!U39</f>
+        <f>VO2max!U39</f>
         <v>4.2591720000000004</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A37">
-        <f>'vo2'!M40</f>
+        <f>VO2max!M40</f>
         <v>165</v>
       </c>
       <c r="B37">
-        <f>'vo2'!T40</f>
+        <f>VO2max!T40</f>
         <v>-0.27328000000000086</v>
       </c>
       <c r="C37">
-        <f>'vo2'!U40</f>
+        <f>VO2max!U40</f>
         <v>5.2264800000000022</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A38">
-        <f>'vo2'!M41</f>
+        <f>VO2max!M41</f>
         <v>167</v>
       </c>
       <c r="B38">
-        <f>'vo2'!T41</f>
+        <f>VO2max!T41</f>
         <v>-0.28098133333333419</v>
       </c>
       <c r="C38">
-        <f>'vo2'!U41</f>
+        <f>VO2max!U41</f>
         <v>5.3737680000000019</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A39">
-        <f>'vo2'!M42</f>
+        <f>VO2max!M42</f>
         <v>169</v>
       </c>
       <c r="B39">
-        <f>'vo2'!T42</f>
+        <f>VO2max!T42</f>
         <v>-0.56072533333333419</v>
       </c>
       <c r="C39">
-        <f>'vo2'!U42</f>
+        <f>VO2max!U42</f>
         <v>5.9927520000000012</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A40">
-        <f>'vo2'!M43</f>
+        <f>VO2max!M43</f>
         <v>173</v>
       </c>
       <c r="B40">
-        <f>'vo2'!T43</f>
+        <f>VO2max!T43</f>
         <v>-0.52176000000000089</v>
       </c>
       <c r="C40">
-        <f>'vo2'!U43</f>
+        <f>VO2max!U43</f>
         <v>5.0871600000000017</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A41">
-        <f>'vo2'!M44</f>
+        <f>VO2max!M44</f>
         <v>170</v>
       </c>
       <c r="B41">
-        <f>'vo2'!T44</f>
+        <f>VO2max!T44</f>
         <v>-0.52518400000000076</v>
       </c>
       <c r="C41">
-        <f>'vo2'!U44</f>
+        <f>VO2max!U44</f>
         <v>5.6129040000000012</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A42">
-        <f>'vo2'!M45</f>
+        <f>VO2max!M45</f>
         <v>161</v>
       </c>
       <c r="B42">
-        <f>'vo2'!T45</f>
+        <f>VO2max!T45</f>
         <v>-0.36332266666666713</v>
       </c>
       <c r="C42">
-        <f>'vo2'!U45</f>
+        <f>VO2max!U45</f>
         <v>3.0469560000000007</v>
       </c>
     </row>
@@ -9724,7 +9732,7 @@
   <dimension ref="A1:C42"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:C1048576"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9734,7 +9742,7 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="str">
-        <f>'vo2'!M4</f>
+        <f>VO2max!M4</f>
         <v>HR
 bpm</v>
       </c>
@@ -9747,575 +9755,575 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2">
-        <f>'vo2'!M5</f>
+        <f>VO2max!M5</f>
         <v>78</v>
       </c>
       <c r="B2">
-        <f>'vo2'!T5*9</f>
+        <f>VO2max!T5*9</f>
         <v>1.9452959999999999</v>
       </c>
       <c r="C2">
-        <f>'vo2'!U5*4</f>
+        <f>VO2max!U5*4</f>
         <v>0.21614400000000022</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3">
-        <f>'vo2'!M6</f>
+        <f>VO2max!M6</f>
         <v>76</v>
       </c>
       <c r="B3">
-        <f>'vo2'!T6*9</f>
+        <f>VO2max!T6*9</f>
         <v>1.2091199999999995</v>
       </c>
       <c r="C3">
-        <f>'vo2'!U6*4</f>
+        <f>VO2max!U6*4</f>
         <v>0.43968000000000046</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4">
-        <f>'vo2'!M7</f>
+        <f>VO2max!M7</f>
         <v>70</v>
       </c>
       <c r="B4">
-        <f>'vo2'!T7*9</f>
+        <f>VO2max!T7*9</f>
         <v>1.3446719999999994</v>
       </c>
       <c r="C4">
-        <f>'vo2'!U7*4</f>
+        <f>VO2max!U7*4</f>
         <v>0.57628800000000047</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5">
-        <f>'vo2'!M8</f>
+        <f>VO2max!M8</f>
         <v>80</v>
       </c>
       <c r="B5">
-        <f>'vo2'!T8*9</f>
+        <f>VO2max!T8*9</f>
         <v>1.4088959999999997</v>
       </c>
       <c r="C5">
-        <f>'vo2'!U8*4</f>
+        <f>VO2max!U8*4</f>
         <v>0.35222400000000031</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6">
-        <f>'vo2'!M9</f>
+        <f>VO2max!M9</f>
         <v>84</v>
       </c>
       <c r="B6">
-        <f>'vo2'!T9*9</f>
+        <f>VO2max!T9*9</f>
         <v>1.6511039999999997</v>
       </c>
       <c r="C6">
-        <f>'vo2'!U9*4</f>
+        <f>VO2max!U9*4</f>
         <v>0.25401600000000041</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7">
-        <f>'vo2'!M10</f>
+        <f>VO2max!M10</f>
         <v>76</v>
       </c>
       <c r="B7">
-        <f>'vo2'!T10*9</f>
+        <f>VO2max!T10*9</f>
         <v>1.7075999999999996</v>
       </c>
       <c r="C7">
-        <f>'vo2'!U10*4</f>
+        <f>VO2max!U10*4</f>
         <v>0.34152000000000032</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8">
-        <f>'vo2'!M11</f>
+        <f>VO2max!M11</f>
         <v>84</v>
       </c>
       <c r="B8">
-        <f>'vo2'!T11*9</f>
+        <f>VO2max!T11*9</f>
         <v>2.9329439999999996</v>
       </c>
       <c r="C8">
-        <f>'vo2'!U11*4</f>
+        <f>VO2max!U11*4</f>
         <v>0.10113599999999996</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9">
-        <f>'vo2'!M12</f>
+        <f>VO2max!M12</f>
         <v>92</v>
       </c>
       <c r="B9">
-        <f>'vo2'!T12*9</f>
+        <f>VO2max!T12*9</f>
         <v>3.5287199999999999</v>
       </c>
       <c r="C9">
-        <f>'vo2'!U12*4</f>
+        <f>VO2max!U12*4</f>
         <v>0.12167999999999997</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10">
-        <f>'vo2'!M13</f>
+        <f>VO2max!M13</f>
         <v>84</v>
       </c>
       <c r="B10">
-        <f>'vo2'!T13*9</f>
+        <f>VO2max!T13*9</f>
         <v>2.809056</v>
       </c>
       <c r="C10">
-        <f>'vo2'!U13*4</f>
+        <f>VO2max!U13*4</f>
         <v>9.6863999999999978E-2</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11">
-        <f>'vo2'!M14</f>
+        <f>VO2max!M14</f>
         <v>82</v>
       </c>
       <c r="B11">
-        <f>'vo2'!T14*9</f>
+        <f>VO2max!T14*9</f>
         <v>3.4027199999999991</v>
       </c>
       <c r="C11">
-        <f>'vo2'!U14*4</f>
+        <f>VO2max!U14*4</f>
         <v>-0.40031999999999923</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12">
-        <f>'vo2'!M15</f>
+        <f>VO2max!M15</f>
         <v>88</v>
       </c>
       <c r="B12">
-        <f>'vo2'!T15*9</f>
+        <f>VO2max!T15*9</f>
         <v>4.8094079999999995</v>
       </c>
       <c r="C12">
-        <f>'vo2'!U15*4</f>
+        <f>VO2max!U15*4</f>
         <v>-0.90988799999999925</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13">
-        <f>'vo2'!M16</f>
+        <f>VO2max!M16</f>
         <v>88</v>
       </c>
       <c r="B13">
-        <f>'vo2'!T16*9</f>
+        <f>VO2max!T16*9</f>
         <v>4.878671999999999</v>
       </c>
       <c r="C13">
-        <f>'vo2'!U16*4</f>
+        <f>VO2max!U16*4</f>
         <v>-0.92299199999999926</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14">
-        <f>'vo2'!M17</f>
+        <f>VO2max!M17</f>
         <v>90</v>
       </c>
       <c r="B14">
-        <f>'vo2'!T17*9</f>
+        <f>VO2max!T17*9</f>
         <v>5.8661279999999998</v>
       </c>
       <c r="C14">
-        <f>'vo2'!U17*4</f>
+        <f>VO2max!U17*4</f>
         <v>-1.1098079999999992</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15">
-        <f>'vo2'!M18</f>
+        <f>VO2max!M18</f>
         <v>94</v>
       </c>
       <c r="B15">
-        <f>'vo2'!T18*9</f>
+        <f>VO2max!T18*9</f>
         <v>5.9334719999999992</v>
       </c>
       <c r="C15">
-        <f>'vo2'!U18*4</f>
+        <f>VO2max!U18*4</f>
         <v>-1.2491519999999996</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16">
-        <f>'vo2'!M19</f>
+        <f>VO2max!M19</f>
         <v>96</v>
       </c>
       <c r="B16">
-        <f>'vo2'!T19*9</f>
+        <f>VO2max!T19*9</f>
         <v>7.9756799999999988</v>
       </c>
       <c r="C16">
-        <f>'vo2'!U19*4</f>
+        <f>VO2max!U19*4</f>
         <v>-1.9939199999999995</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17">
-        <f>'vo2'!M20</f>
+        <f>VO2max!M20</f>
         <v>99</v>
       </c>
       <c r="B17">
-        <f>'vo2'!T20*9</f>
+        <f>VO2max!T20*9</f>
         <v>9.7514400000000006</v>
       </c>
       <c r="C17">
-        <f>'vo2'!U20*4</f>
+        <f>VO2max!U20*4</f>
         <v>-2.6162400000000003</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18">
-        <f>'vo2'!M21</f>
+        <f>VO2max!M21</f>
         <v>102</v>
       </c>
       <c r="B18">
-        <f>'vo2'!T21*9</f>
+        <f>VO2max!T21*9</f>
         <v>9.1929599999999994</v>
       </c>
       <c r="C18">
-        <f>'vo2'!U21*4</f>
+        <f>VO2max!U21*4</f>
         <v>-2.2982399999999998</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19">
-        <f>'vo2'!M22</f>
+        <f>VO2max!M22</f>
         <v>103</v>
       </c>
       <c r="B19">
-        <f>'vo2'!T22*9</f>
+        <f>VO2max!T22*9</f>
         <v>11.114880000000003</v>
       </c>
       <c r="C19">
-        <f>'vo2'!U22*4</f>
+        <f>VO2max!U22*4</f>
         <v>-2.7787199999999999</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20">
-        <f>'vo2'!M23</f>
+        <f>VO2max!M23</f>
         <v>106</v>
       </c>
       <c r="B20">
-        <f>'vo2'!T23*9</f>
+        <f>VO2max!T23*9</f>
         <v>10.528128000000002</v>
       </c>
       <c r="C20">
-        <f>'vo2'!U23*4</f>
+        <f>VO2max!U23*4</f>
         <v>-2.2164479999999998</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21">
-        <f>'vo2'!M24</f>
+        <f>VO2max!M24</f>
         <v>114</v>
       </c>
       <c r="B21">
-        <f>'vo2'!T24*9</f>
+        <f>VO2max!T24*9</f>
         <v>8.8490879999999983</v>
       </c>
       <c r="C21">
-        <f>'vo2'!U24*4</f>
+        <f>VO2max!U24*4</f>
         <v>-1.4748479999999982</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22">
-        <f>'vo2'!M25</f>
+        <f>VO2max!M25</f>
         <v>106</v>
       </c>
       <c r="B22">
-        <f>'vo2'!T25*9</f>
+        <f>VO2max!T25*9</f>
         <v>9.9859199999999984</v>
       </c>
       <c r="C22">
-        <f>'vo2'!U25*4</f>
+        <f>VO2max!U25*4</f>
         <v>-1.4265599999999987</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23">
-        <f>'vo2'!M26</f>
+        <f>VO2max!M26</f>
         <v>109</v>
       </c>
       <c r="B23">
-        <f>'vo2'!T26*9</f>
+        <f>VO2max!T26*9</f>
         <v>11.872559999999998</v>
       </c>
       <c r="C23">
-        <f>'vo2'!U26*4</f>
+        <f>VO2max!U26*4</f>
         <v>-1.6960799999999985</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24">
-        <f>'vo2'!M27</f>
+        <f>VO2max!M27</f>
         <v>117</v>
       </c>
       <c r="B24">
-        <f>'vo2'!T27*9</f>
+        <f>VO2max!T27*9</f>
         <v>10.959839999999998</v>
       </c>
       <c r="C24">
-        <f>'vo2'!U27*4</f>
+        <f>VO2max!U27*4</f>
         <v>0</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25">
-        <f>'vo2'!M28</f>
+        <f>VO2max!M28</f>
         <v>124</v>
       </c>
       <c r="B25">
-        <f>'vo2'!T28*9</f>
+        <f>VO2max!T28*9</f>
         <v>10.771055999999998</v>
       </c>
       <c r="C25">
-        <f>'vo2'!U28*4</f>
+        <f>VO2max!U28*4</f>
         <v>1.196784000000001</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26">
-        <f>'vo2'!M29</f>
+        <f>VO2max!M29</f>
         <v>126</v>
       </c>
       <c r="B26">
-        <f>'vo2'!T29*9</f>
+        <f>VO2max!T29*9</f>
         <v>9.178799999999999</v>
       </c>
       <c r="C26">
-        <f>'vo2'!U29*4</f>
+        <f>VO2max!U29*4</f>
         <v>1.8357600000000023</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27">
-        <f>'vo2'!M30</f>
+        <f>VO2max!M30</f>
         <v>129</v>
       </c>
       <c r="B27">
-        <f>'vo2'!T30*9</f>
+        <f>VO2max!T30*9</f>
         <v>9.6455999999999964</v>
       </c>
       <c r="C27">
-        <f>'vo2'!U30*4</f>
+        <f>VO2max!U30*4</f>
         <v>1.9291200000000019</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28">
-        <f>'vo2'!M31</f>
+        <f>VO2max!M31</f>
         <v>135</v>
       </c>
       <c r="B28">
-        <f>'vo2'!T31*9</f>
+        <f>VO2max!T31*9</f>
         <v>10.481375999999996</v>
       </c>
       <c r="C28">
-        <f>'vo2'!U31*4</f>
+        <f>VO2max!U31*4</f>
         <v>3.1899840000000039</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29">
-        <f>'vo2'!M32</f>
+        <f>VO2max!M32</f>
         <v>138</v>
       </c>
       <c r="B29">
-        <f>'vo2'!T32*9</f>
+        <f>VO2max!T32*9</f>
         <v>7.8321599999999991</v>
       </c>
       <c r="C29">
-        <f>'vo2'!U32*4</f>
+        <f>VO2max!U32*4</f>
         <v>5.2214400000000003</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30">
-        <f>'vo2'!M33</f>
+        <f>VO2max!M33</f>
         <v>148</v>
       </c>
       <c r="B30">
-        <f>'vo2'!T33*9</f>
+        <f>VO2max!T33*9</f>
         <v>8.0180159999999994</v>
       </c>
       <c r="C30">
-        <f>'vo2'!U33*4</f>
+        <f>VO2max!U33*4</f>
         <v>6.131424</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31">
-        <f>'vo2'!M34</f>
+        <f>VO2max!M34</f>
         <v>139</v>
       </c>
       <c r="B31">
-        <f>'vo2'!T34*9</f>
+        <f>VO2max!T34*9</f>
         <v>6.9573119999999991</v>
       </c>
       <c r="C31">
-        <f>'vo2'!U34*4</f>
+        <f>VO2max!U34*4</f>
         <v>6.0876480000000024</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32">
-        <f>'vo2'!M35</f>
+        <f>VO2max!M35</f>
         <v>143</v>
       </c>
       <c r="B32">
-        <f>'vo2'!T35*9</f>
+        <f>VO2max!T35*9</f>
         <v>8.2974719999999973</v>
       </c>
       <c r="C32">
-        <f>'vo2'!U35*4</f>
+        <f>VO2max!U35*4</f>
         <v>7.2602880000000019</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33">
-        <f>'vo2'!M36</f>
+        <f>VO2max!M36</f>
         <v>149</v>
       </c>
       <c r="B33">
-        <f>'vo2'!T36*9</f>
+        <f>VO2max!T36*9</f>
         <v>5.2545599999999952</v>
       </c>
       <c r="C33">
-        <f>'vo2'!U36*4</f>
+        <f>VO2max!U36*4</f>
         <v>10.509120000000005</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A34">
-        <f>'vo2'!M37</f>
+        <f>VO2max!M37</f>
         <v>155</v>
       </c>
       <c r="B34">
-        <f>'vo2'!T37*9</f>
+        <f>VO2max!T37*9</f>
         <v>3.7339679999999928</v>
       </c>
       <c r="C34">
-        <f>'vo2'!U37*4</f>
+        <f>VO2max!U37*4</f>
         <v>12.268752000000003</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A35">
-        <f>'vo2'!M38</f>
+        <f>VO2max!M38</f>
         <v>158</v>
       </c>
       <c r="B35">
-        <f>'vo2'!T38*9</f>
+        <f>VO2max!T38*9</f>
         <v>2.3767679999999993</v>
       </c>
       <c r="C35">
-        <f>'vo2'!U38*4</f>
+        <f>VO2max!U38*4</f>
         <v>15.448992000000002</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A36">
-        <f>'vo2'!M39</f>
+        <f>VO2max!M39</f>
         <v>161</v>
       </c>
       <c r="B36">
-        <f>'vo2'!T39*9</f>
+        <f>VO2max!T39*9</f>
         <v>0.58747199999999777</v>
       </c>
       <c r="C36">
-        <f>'vo2'!U39*4</f>
+        <f>VO2max!U39*4</f>
         <v>17.036688000000002</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A37">
-        <f>'vo2'!M40</f>
+        <f>VO2max!M40</f>
         <v>165</v>
       </c>
       <c r="B37">
-        <f>'vo2'!T40*9</f>
+        <f>VO2max!T40*9</f>
         <v>-2.4595200000000075</v>
       </c>
       <c r="C37">
-        <f>'vo2'!U40*4</f>
+        <f>VO2max!U40*4</f>
         <v>20.905920000000009</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A38">
-        <f>'vo2'!M41</f>
+        <f>VO2max!M41</f>
         <v>167</v>
       </c>
       <c r="B38">
-        <f>'vo2'!T41*9</f>
+        <f>VO2max!T41*9</f>
         <v>-2.5288320000000075</v>
       </c>
       <c r="C38">
-        <f>'vo2'!U41*4</f>
+        <f>VO2max!U41*4</f>
         <v>21.495072000000008</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A39">
-        <f>'vo2'!M42</f>
+        <f>VO2max!M42</f>
         <v>169</v>
       </c>
       <c r="B39">
-        <f>'vo2'!T42*9</f>
+        <f>VO2max!T42*9</f>
         <v>-5.0465280000000075</v>
       </c>
       <c r="C39">
-        <f>'vo2'!U42*4</f>
+        <f>VO2max!U42*4</f>
         <v>23.971008000000005</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A40">
-        <f>'vo2'!M43</f>
+        <f>VO2max!M43</f>
         <v>173</v>
       </c>
       <c r="B40">
-        <f>'vo2'!T43*9</f>
+        <f>VO2max!T43*9</f>
         <v>-4.6958400000000076</v>
       </c>
       <c r="C40">
-        <f>'vo2'!U43*4</f>
+        <f>VO2max!U43*4</f>
         <v>20.348640000000007</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A41">
-        <f>'vo2'!M44</f>
+        <f>VO2max!M44</f>
         <v>170</v>
       </c>
       <c r="B41">
-        <f>'vo2'!T44*9</f>
+        <f>VO2max!T44*9</f>
         <v>-4.7266560000000073</v>
       </c>
       <c r="C41">
-        <f>'vo2'!U44*4</f>
+        <f>VO2max!U44*4</f>
         <v>22.451616000000005</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A42">
-        <f>'vo2'!M45</f>
+        <f>VO2max!M45</f>
         <v>161</v>
       </c>
       <c r="B42">
-        <f>'vo2'!T45*9</f>
+        <f>VO2max!T45*9</f>
         <v>-3.2699040000000039</v>
       </c>
       <c r="C42">
-        <f>'vo2'!U45*4</f>
+        <f>VO2max!U45*4</f>
         <v>12.187824000000003</v>
       </c>
     </row>
@@ -10330,7 +10338,7 @@
   <dimension ref="A1:C38"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:C1048576"/>
+      <selection activeCell="L33" sqref="L33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -10342,7 +10350,7 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="str">
-        <f>'vo2'!W4</f>
+        <f>VO2max!W4</f>
         <v>%VO2max</v>
       </c>
       <c r="B1" t="s">
@@ -10354,519 +10362,519 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="4">
-        <f>'vo2'!W5</f>
+        <f>VO2max!W5</f>
         <v>0.12280701754385964</v>
       </c>
       <c r="B2">
-        <f>'vo2'!T5*9</f>
+        <f>VO2max!T5*9</f>
         <v>1.9452959999999999</v>
       </c>
       <c r="C2">
-        <f>'vo2'!U5*4</f>
+        <f>VO2max!U5*4</f>
         <v>0.21614400000000022</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="4">
-        <f>'vo2'!W6</f>
+        <f>VO2max!W6</f>
         <v>9.0643274853801165E-2</v>
       </c>
       <c r="B3">
-        <f>'vo2'!T6*9</f>
+        <f>VO2max!T6*9</f>
         <v>1.2091199999999995</v>
       </c>
       <c r="C3">
-        <f>'vo2'!U6*4</f>
+        <f>VO2max!U6*4</f>
         <v>0.43968000000000046</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="4">
-        <f>'vo2'!W7</f>
+        <f>VO2max!W7</f>
         <v>0.10818713450292397</v>
       </c>
       <c r="B4">
-        <f>'vo2'!T7*9</f>
+        <f>VO2max!T7*9</f>
         <v>1.3446719999999994</v>
       </c>
       <c r="C4">
-        <f>'vo2'!U7*4</f>
+        <f>VO2max!U7*4</f>
         <v>0.57628800000000047</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="4">
-        <f>'vo2'!W8</f>
+        <f>VO2max!W8</f>
         <v>9.6491228070175419E-2</v>
       </c>
       <c r="B5">
-        <f>'vo2'!T8*9</f>
+        <f>VO2max!T8*9</f>
         <v>1.4088959999999997</v>
       </c>
       <c r="C5">
-        <f>'vo2'!U8*4</f>
+        <f>VO2max!U8*4</f>
         <v>0.35222400000000031</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="4">
-        <f>'vo2'!W9</f>
+        <f>VO2max!W9</f>
         <v>0.10526315789473684</v>
       </c>
       <c r="B6">
-        <f>'vo2'!T9*9</f>
+        <f>VO2max!T9*9</f>
         <v>1.6511039999999997</v>
       </c>
       <c r="C6">
-        <f>'vo2'!U9*4</f>
+        <f>VO2max!U9*4</f>
         <v>0.25401600000000041</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="4">
-        <f>'vo2'!W10</f>
+        <f>VO2max!W10</f>
         <v>0.11695906432748537</v>
       </c>
       <c r="B7">
-        <f>'vo2'!T10*9</f>
+        <f>VO2max!T10*9</f>
         <v>1.7075999999999996</v>
       </c>
       <c r="C7">
-        <f>'vo2'!U10*4</f>
+        <f>VO2max!U10*4</f>
         <v>0.34152000000000032</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="4">
-        <f>'vo2'!W11</f>
+        <f>VO2max!W11</f>
         <v>0.17251461988304093</v>
       </c>
       <c r="B8">
-        <f>'vo2'!T11*9</f>
+        <f>VO2max!T11*9</f>
         <v>2.9329439999999996</v>
       </c>
       <c r="C8">
-        <f>'vo2'!U11*4</f>
+        <f>VO2max!U11*4</f>
         <v>0.10113599999999996</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" s="4">
-        <f>'vo2'!W12</f>
+        <f>VO2max!W12</f>
         <v>0.20760233918128651</v>
       </c>
       <c r="B9">
-        <f>'vo2'!T12*9</f>
+        <f>VO2max!T12*9</f>
         <v>3.5287199999999999</v>
       </c>
       <c r="C9">
-        <f>'vo2'!U12*4</f>
+        <f>VO2max!U12*4</f>
         <v>0.12167999999999997</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" s="4">
-        <f>'vo2'!W13</f>
+        <f>VO2max!W13</f>
         <v>0.16666666666666666</v>
       </c>
       <c r="B10">
-        <f>'vo2'!T13*9</f>
+        <f>VO2max!T13*9</f>
         <v>2.809056</v>
       </c>
       <c r="C10">
-        <f>'vo2'!U13*4</f>
+        <f>VO2max!U13*4</f>
         <v>9.6863999999999978E-2</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" s="4">
-        <f>'vo2'!W14</f>
+        <f>VO2max!W14</f>
         <v>0.17251461988304093</v>
       </c>
       <c r="B11">
-        <f>'vo2'!T14*9</f>
+        <f>VO2max!T14*9</f>
         <v>3.4027199999999991</v>
       </c>
       <c r="C11">
-        <f>'vo2'!U14*4</f>
+        <f>VO2max!U14*4</f>
         <v>-0.40031999999999923</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" s="4">
-        <f>'vo2'!W15</f>
+        <f>VO2max!W15</f>
         <v>0.22807017543859648</v>
       </c>
       <c r="B12">
-        <f>'vo2'!T15*9</f>
+        <f>VO2max!T15*9</f>
         <v>4.8094079999999995</v>
       </c>
       <c r="C12">
-        <f>'vo2'!U15*4</f>
+        <f>VO2max!U15*4</f>
         <v>-0.90988799999999925</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" s="4">
-        <f>'vo2'!W16</f>
+        <f>VO2max!W16</f>
         <v>0.22807017543859648</v>
       </c>
       <c r="B13">
-        <f>'vo2'!T16*9</f>
+        <f>VO2max!T16*9</f>
         <v>4.878671999999999</v>
       </c>
       <c r="C13">
-        <f>'vo2'!U16*4</f>
+        <f>VO2max!U16*4</f>
         <v>-0.92299199999999926</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" s="4">
-        <f>'vo2'!W17</f>
+        <f>VO2max!W17</f>
         <v>0.27777777777777773</v>
       </c>
       <c r="B14">
-        <f>'vo2'!T17*9</f>
+        <f>VO2max!T17*9</f>
         <v>5.8661279999999998</v>
       </c>
       <c r="C14">
-        <f>'vo2'!U17*4</f>
+        <f>VO2max!U17*4</f>
         <v>-1.1098079999999992</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" s="4">
-        <f>'vo2'!W18</f>
+        <f>VO2max!W18</f>
         <v>0.27192982456140352</v>
       </c>
       <c r="B15">
-        <f>'vo2'!T18*9</f>
+        <f>VO2max!T18*9</f>
         <v>5.9334719999999992</v>
       </c>
       <c r="C15">
-        <f>'vo2'!U18*4</f>
+        <f>VO2max!U18*4</f>
         <v>-1.2491519999999996</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" s="4">
-        <f>'vo2'!W19</f>
+        <f>VO2max!W19</f>
         <v>0.34795321637426901</v>
       </c>
       <c r="B16">
-        <f>'vo2'!T19*9</f>
+        <f>VO2max!T19*9</f>
         <v>7.9756799999999988</v>
       </c>
       <c r="C16">
-        <f>'vo2'!U19*4</f>
+        <f>VO2max!U19*4</f>
         <v>-1.9939199999999995</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" s="4">
-        <f>'vo2'!W20</f>
+        <f>VO2max!W20</f>
         <v>0.41812865497076024</v>
       </c>
       <c r="B17">
-        <f>'vo2'!T20*9</f>
+        <f>VO2max!T20*9</f>
         <v>9.7514400000000006</v>
       </c>
       <c r="C17">
-        <f>'vo2'!U20*4</f>
+        <f>VO2max!U20*4</f>
         <v>-2.6162400000000003</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" s="4">
-        <f>'vo2'!W21</f>
+        <f>VO2max!W21</f>
         <v>0.40350877192982454</v>
       </c>
       <c r="B18">
-        <f>'vo2'!T21*9</f>
+        <f>VO2max!T21*9</f>
         <v>9.1929599999999994</v>
       </c>
       <c r="C18">
-        <f>'vo2'!U21*4</f>
+        <f>VO2max!U21*4</f>
         <v>-2.2982399999999998</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" s="4">
-        <f>'vo2'!W22</f>
+        <f>VO2max!W22</f>
         <v>0.48538011695906436</v>
       </c>
       <c r="B19">
-        <f>'vo2'!T22*9</f>
+        <f>VO2max!T22*9</f>
         <v>11.114880000000003</v>
       </c>
       <c r="C19">
-        <f>'vo2'!U22*4</f>
+        <f>VO2max!U22*4</f>
         <v>-2.7787199999999999</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" s="4">
-        <f>'vo2'!W23</f>
+        <f>VO2max!W23</f>
         <v>0.48245614035087714</v>
       </c>
       <c r="B20">
-        <f>'vo2'!T23*9</f>
+        <f>VO2max!T23*9</f>
         <v>10.528128000000002</v>
       </c>
       <c r="C20">
-        <f>'vo2'!U23*4</f>
+        <f>VO2max!U23*4</f>
         <v>-2.2164479999999998</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" s="4">
-        <f>'vo2'!W24</f>
+        <f>VO2max!W24</f>
         <v>0.42690058479532161</v>
       </c>
       <c r="B21">
-        <f>'vo2'!T24*9</f>
+        <f>VO2max!T24*9</f>
         <v>8.8490879999999983</v>
       </c>
       <c r="C21">
-        <f>'vo2'!U24*4</f>
+        <f>VO2max!U24*4</f>
         <v>-1.4748479999999982</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" s="4">
-        <f>'vo2'!W25</f>
+        <f>VO2max!W25</f>
         <v>0.49122807017543857</v>
       </c>
       <c r="B22">
-        <f>'vo2'!T25*9</f>
+        <f>VO2max!T25*9</f>
         <v>9.9859199999999984</v>
       </c>
       <c r="C22">
-        <f>'vo2'!U25*4</f>
+        <f>VO2max!U25*4</f>
         <v>-1.4265599999999987</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" s="4">
-        <f>'vo2'!W26</f>
+        <f>VO2max!W26</f>
         <v>0.58771929824561397</v>
       </c>
       <c r="B23">
-        <f>'vo2'!T26*9</f>
+        <f>VO2max!T26*9</f>
         <v>11.872559999999998</v>
       </c>
       <c r="C23">
-        <f>'vo2'!U26*4</f>
+        <f>VO2max!U26*4</f>
         <v>-1.6960799999999985</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" s="4">
-        <f>'vo2'!W27</f>
+        <f>VO2max!W27</f>
         <v>0.62573099415204669</v>
       </c>
       <c r="B24">
-        <f>'vo2'!T27*9</f>
+        <f>VO2max!T27*9</f>
         <v>10.959839999999998</v>
       </c>
       <c r="C24">
-        <f>'vo2'!U27*4</f>
+        <f>VO2max!U27*4</f>
         <v>0</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" s="4">
-        <f>'vo2'!W28</f>
+        <f>VO2max!W28</f>
         <v>0.67836257309941517</v>
       </c>
       <c r="B25">
-        <f>'vo2'!T28*9</f>
+        <f>VO2max!T28*9</f>
         <v>10.771055999999998</v>
       </c>
       <c r="C25">
-        <f>'vo2'!U28*4</f>
+        <f>VO2max!U28*4</f>
         <v>1.196784000000001</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" s="4">
-        <f>'vo2'!W29</f>
+        <f>VO2max!W29</f>
         <v>0.62280701754385959</v>
       </c>
       <c r="B26">
-        <f>'vo2'!T29*9</f>
+        <f>VO2max!T29*9</f>
         <v>9.178799999999999</v>
       </c>
       <c r="C26">
-        <f>'vo2'!U29*4</f>
+        <f>VO2max!U29*4</f>
         <v>1.8357600000000023</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" s="4">
-        <f>'vo2'!W30</f>
+        <f>VO2max!W30</f>
         <v>0.64912280701754377</v>
       </c>
       <c r="B27">
-        <f>'vo2'!T30*9</f>
+        <f>VO2max!T30*9</f>
         <v>9.6455999999999964</v>
       </c>
       <c r="C27">
-        <f>'vo2'!U30*4</f>
+        <f>VO2max!U30*4</f>
         <v>1.9291200000000019</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" s="4">
-        <f>'vo2'!W31</f>
+        <f>VO2max!W31</f>
         <v>0.76608187134502914</v>
       </c>
       <c r="B28">
-        <f>'vo2'!T31*9</f>
+        <f>VO2max!T31*9</f>
         <v>10.481375999999996</v>
       </c>
       <c r="C28">
-        <f>'vo2'!U31*4</f>
+        <f>VO2max!U31*4</f>
         <v>3.1899840000000039</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29" s="4">
-        <f>'vo2'!W32</f>
+        <f>VO2max!W32</f>
         <v>0.72514619883040932</v>
       </c>
       <c r="B29">
-        <f>'vo2'!T32*9</f>
+        <f>VO2max!T32*9</f>
         <v>7.8321599999999991</v>
       </c>
       <c r="C29">
-        <f>'vo2'!U32*4</f>
+        <f>VO2max!U32*4</f>
         <v>5.2214400000000003</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30" s="4">
-        <f>'vo2'!W33</f>
+        <f>VO2max!W33</f>
         <v>0.78070175438596479</v>
       </c>
       <c r="B30">
-        <f>'vo2'!T33*9</f>
+        <f>VO2max!T33*9</f>
         <v>8.0180159999999994</v>
       </c>
       <c r="C30">
-        <f>'vo2'!U33*4</f>
+        <f>VO2max!U33*4</f>
         <v>6.131424</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31" s="4">
-        <f>'vo2'!W34</f>
+        <f>VO2max!W34</f>
         <v>0.7192982456140351</v>
       </c>
       <c r="B31">
-        <f>'vo2'!T34*9</f>
+        <f>VO2max!T34*9</f>
         <v>6.9573119999999991</v>
       </c>
       <c r="C31">
-        <f>'vo2'!U34*4</f>
+        <f>VO2max!U34*4</f>
         <v>6.0876480000000024</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32" s="4">
-        <f>'vo2'!W35</f>
+        <f>VO2max!W35</f>
         <v>0.85964912280701744</v>
       </c>
       <c r="B32">
-        <f>'vo2'!T35*9</f>
+        <f>VO2max!T35*9</f>
         <v>8.2974719999999973</v>
       </c>
       <c r="C32">
-        <f>'vo2'!U35*4</f>
+        <f>VO2max!U35*4</f>
         <v>7.2602880000000019</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33" s="4">
-        <f>'vo2'!W36</f>
+        <f>VO2max!W36</f>
         <v>0.85964912280701744</v>
       </c>
       <c r="B33">
-        <f>'vo2'!T36*9</f>
+        <f>VO2max!T36*9</f>
         <v>5.2545599999999952</v>
       </c>
       <c r="C33">
-        <f>'vo2'!U36*4</f>
+        <f>VO2max!U36*4</f>
         <v>10.509120000000005</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A34" s="4">
-        <f>'vo2'!W37</f>
+        <f>VO2max!W37</f>
         <v>0.86257309941520466</v>
       </c>
       <c r="B34">
-        <f>'vo2'!T37*9</f>
+        <f>VO2max!T37*9</f>
         <v>3.7339679999999928</v>
       </c>
       <c r="C34">
-        <f>'vo2'!U37*4</f>
+        <f>VO2max!U37*4</f>
         <v>12.268752000000003</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A35" s="4">
-        <f>'vo2'!W38</f>
+        <f>VO2max!W38</f>
         <v>0.95614035087719296</v>
       </c>
       <c r="B35">
-        <f>'vo2'!T38*9</f>
+        <f>VO2max!T38*9</f>
         <v>2.3767679999999993</v>
       </c>
       <c r="C35">
-        <f>'vo2'!U38*4</f>
+        <f>VO2max!U38*4</f>
         <v>15.448992000000002</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A36" s="4">
-        <f>'vo2'!W39</f>
+        <f>VO2max!W39</f>
         <v>0.9385964912280701</v>
       </c>
       <c r="B36">
-        <f>'vo2'!T39*9</f>
+        <f>VO2max!T39*9</f>
         <v>0.58747199999999777</v>
       </c>
       <c r="C36">
-        <f>'vo2'!U39*4</f>
+        <f>VO2max!U39*4</f>
         <v>17.036688000000002</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A37" s="4">
-        <f>'vo2'!W40</f>
+        <f>VO2max!W40</f>
         <v>0.97076023391812871</v>
       </c>
       <c r="B37">
-        <f>'vo2'!T40*9</f>
+        <f>VO2max!T40*9</f>
         <v>-2.4595200000000075</v>
       </c>
       <c r="C37">
-        <f>'vo2'!U40*4</f>
+        <f>VO2max!U40*4</f>
         <v>20.905920000000009</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A38" s="4">
-        <f>'vo2'!W41</f>
+        <f>VO2max!W41</f>
         <v>1</v>
       </c>
       <c r="B38">
-        <f>'vo2'!T41*9</f>
+        <f>VO2max!T41*9</f>
         <v>-2.5288320000000075</v>
       </c>
       <c r="C38">
-        <f>'vo2'!U41*4</f>
+        <f>VO2max!U41*4</f>
         <v>21.495072000000008</v>
       </c>
     </row>

</xml_diff>